<commit_message>
updated spreadsheet containing the best parameters and their accuracies
</commit_message>
<xml_diff>
--- a/executions-best-parameters.xlsx
+++ b/executions-best-parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="54280" yWindow="10200" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="51440" yWindow="9960" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Dataset</t>
   </si>
@@ -129,6 +129,21 @@
   </si>
   <si>
     <t>minimum accur with maximum differ  less than 0.01</t>
+  </si>
+  <si>
+    <t>minPredictionRario is the mean. We get the best accuracy for  6 to 9 with a stdev = 2.63</t>
+  </si>
+  <si>
+    <t>average accuracy 0.117</t>
+  </si>
+  <si>
+    <t>minPredictionRatio = [1,3] and noiseRatio = [0.8, 1]</t>
+  </si>
+  <si>
+    <t>minPredictionRatio = [3,7]</t>
+  </si>
+  <si>
+    <t>the parameters chosen by TED weren't optimal - also I got less than the reported accuracy</t>
   </si>
 </sst>
 </file>
@@ -174,12 +189,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -191,7 +218,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -213,15 +240,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -232,6 +276,11 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -242,6 +291,11 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -520,7 +574,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,6 +582,8 @@
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="6" width="33.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -559,33 +615,36 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
+    <row r="2" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
         <v>4865</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="6">
         <v>494</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="6">
         <v>11.227955</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="6">
         <v>11.227955</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
         <v>0.37</v>
       </c>
-      <c r="H2" s="2">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1</v>
+      <c r="H2" s="6">
+        <v>3</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -616,6 +675,9 @@
       <c r="I3" s="2">
         <v>1</v>
       </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -666,70 +728,73 @@
         <v>1.2334445730000001</v>
       </c>
       <c r="G5" s="2">
-        <v>0.224</v>
+        <v>0.23</v>
       </c>
       <c r="H5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>5000</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="10">
+        <v>5000</v>
+      </c>
+      <c r="C6" s="10">
         <v>74</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="10">
         <v>133.01</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="10">
         <v>26.063800000000001</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="10">
         <v>5.1032466489999999</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="10">
         <v>0.8</v>
       </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="10">
         <v>45000</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="10">
         <v>22422</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="10">
         <v>28.425312000000002</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="10">
         <v>28.4252</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="10">
         <v>1.0000039089999999</v>
       </c>
-      <c r="G7" s="2">
-        <v>0.41</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="G7" s="10">
+        <v>0.42</v>
+      </c>
+      <c r="H7" s="10">
+        <v>2</v>
+      </c>
+      <c r="I7" s="10">
         <v>1</v>
       </c>
     </row>
@@ -858,32 +923,32 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
-        <v>5000</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C12" s="4">
         <v>10</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <v>42.677799999999998</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="4">
         <v>8.9474</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="4">
         <v>4.7698549300000002</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="4">
         <v>0.26700000000000002</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="4">
         <v>9</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="4">
         <v>0.3</v>
       </c>
       <c r="J12" s="3" t="s">
@@ -910,7 +975,7 @@
         <v>1.199915329</v>
       </c>
       <c r="G13" s="2">
-        <v>0.55418210000000001</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
@@ -919,32 +984,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
-        <v>5000</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C14" s="4">
         <v>48</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="4">
         <v>119.9794</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="4">
         <v>22.779599999999999</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="4">
         <v>5.2669669350000001</v>
       </c>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2">
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
         <v>1</v>
       </c>
       <c r="J14" s="3" t="s">
@@ -971,7 +1036,7 @@
         <v>2.665813816</v>
       </c>
       <c r="G15" s="2">
-        <v>0.26494267999999999</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H15" s="2">
         <v>0</v>
@@ -980,39 +1045,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
-        <v>5000</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B16" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C16" s="4">
         <v>20</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <v>59.182600000000001</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <v>16.541799999999999</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <v>3.5777605819999998</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="4">
         <v>0.54920000000000002</v>
       </c>
-      <c r="H16" s="2">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2">
+      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
         <v>1</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1032,7 +1097,7 @@
         <v>2.5714123359999999</v>
       </c>
       <c r="G17" s="2">
-        <v>0.40560000000000002</v>
+        <v>0.45</v>
       </c>
       <c r="H17" s="2">
         <v>0</v>
@@ -1041,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1061,7 +1126,7 @@
         <v>4.8056964940000002</v>
       </c>
       <c r="G18" s="2">
-        <v>0.45190429999999998</v>
+        <v>0.54</v>
       </c>
       <c r="H18" s="2">
         <v>0</v>
@@ -1070,94 +1135,103 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
-        <v>5000</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B19" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C19" s="4">
         <v>20</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="4">
         <v>35.518799999999999</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="4">
         <v>15.850199999999999</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="4">
         <v>2.2409054780000002</v>
       </c>
-      <c r="G19" s="2">
-        <v>0.88339999999999996</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="G19" s="4">
+        <v>1</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
-        <v>5000</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="6">
+        <v>5000</v>
+      </c>
+      <c r="C20" s="6">
         <v>2546</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="6">
         <v>12.079599999999999</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="6">
         <v>10.855600000000001</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="6">
         <v>1.112752865</v>
       </c>
-      <c r="G20" s="2">
-        <v>0.87839999999999996</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="G20" s="6">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="H20" s="6">
+        <v>6</v>
+      </c>
+      <c r="I20" s="6">
+        <v>1</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
-        <v>5000</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B21" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C21" s="4">
         <v>21</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="4">
         <v>33.040399999999998</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="4">
         <v>14.0284</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="4">
         <v>2.3552507770000002</v>
       </c>
-      <c r="G21" s="2">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
-      <c r="I21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G21" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H21" s="4">
+        <v>2</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1177,16 +1251,16 @@
         <v>1.144251355</v>
       </c>
       <c r="G22" s="2">
-        <v>0.32879999999999998</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="H22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1206,7 +1280,7 @@
         <v>3.2971278480000001</v>
       </c>
       <c r="G23" s="2">
-        <v>0.46479999999999999</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="H23" s="2">
         <v>1</v>
@@ -1215,7 +1289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1235,13 +1309,13 @@
         <v>2.375155876</v>
       </c>
       <c r="G24" s="2">
-        <v>0.18260000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="H24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated spreadsheet once again
</commit_message>
<xml_diff>
--- a/executions-best-parameters.xlsx
+++ b/executions-best-parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="51440" yWindow="9960" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="54080" yWindow="9760" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Dataset</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>the parameters chosen by TED weren't optimal - also I got less than the reported accuracy</t>
+  </si>
+  <si>
+    <t>#occurence_on_sequence stdev</t>
   </si>
 </sst>
 </file>
@@ -251,7 +254,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -259,11 +262,14 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -571,22 +577,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="33.83203125" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="6" max="7" width="33.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,48 +612,54 @@
         <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6">
+    <row r="2" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
         <v>4865</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="12">
         <v>494</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="12">
         <v>11.227955</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="12">
         <v>11.227955</v>
       </c>
-      <c r="F2" s="6">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6">
+      <c r="F2" s="12">
+        <v>1</v>
+      </c>
+      <c r="G2" s="12">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12">
         <v>0.37</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="12">
         <v>3</v>
       </c>
-      <c r="I2" s="6">
-        <v>1</v>
-      </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="12">
+        <v>1</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -667,19 +679,22 @@
         <v>1.7887290549999999</v>
       </c>
       <c r="G3" s="2">
+        <v>1.23033395168528</v>
+      </c>
+      <c r="H3" s="2">
         <v>0.33</v>
       </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
       <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -699,16 +714,19 @@
         <v>2.2678774599999998</v>
       </c>
       <c r="G4" s="2">
+        <v>2.35112632441753</v>
+      </c>
+      <c r="H4" s="2">
         <v>0.59</v>
       </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
       <c r="I4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -728,77 +746,86 @@
         <v>1.2334445730000001</v>
       </c>
       <c r="G5" s="2">
+        <v>0.75869833473772297</v>
+      </c>
+      <c r="H5" s="2">
         <v>0.23</v>
       </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
       <c r="I5" s="2">
         <v>1</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="10">
-        <v>5000</v>
-      </c>
-      <c r="C6" s="10">
+      <c r="B6" s="9">
+        <v>5000</v>
+      </c>
+      <c r="C6" s="9">
         <v>74</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>133.01</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>26.063800000000001</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>5.1032466489999999</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
+        <v>6.1603756712864302</v>
+      </c>
+      <c r="H6" s="9">
         <v>0.8</v>
       </c>
-      <c r="H6" s="10">
-        <v>0</v>
-      </c>
-      <c r="I6" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>45000</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>22422</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>28.425312000000002</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>28.4252</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>1.0000039089999999</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
+        <v>1.9770885999336701E-3</v>
+      </c>
+      <c r="H7" s="9">
         <v>0.42</v>
       </c>
-      <c r="H7" s="10">
+      <c r="I7" s="9">
         <v>2</v>
       </c>
-      <c r="I7" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -818,16 +845,19 @@
         <v>1.040882702</v>
       </c>
       <c r="G8" s="2">
+        <v>0.28774541660017799</v>
+      </c>
+      <c r="H8" s="2">
         <v>0.35</v>
       </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
       <c r="I8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -847,19 +877,22 @@
         <v>3.2972347630000001</v>
       </c>
       <c r="G9" s="4">
+        <v>2.3277143734745902</v>
+      </c>
+      <c r="H9" s="4">
         <v>0.67759999999999998</v>
       </c>
-      <c r="H9" s="4">
-        <v>1</v>
-      </c>
       <c r="I9" s="4">
         <v>1</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -879,19 +912,22 @@
         <v>2.938521707</v>
       </c>
       <c r="G10" s="4">
+        <v>2.5912114762874499</v>
+      </c>
+      <c r="H10" s="4">
         <v>0.26879999999999998</v>
       </c>
-      <c r="H10" s="4">
-        <v>1</v>
-      </c>
       <c r="I10" s="4">
         <v>1</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -911,19 +947,22 @@
         <v>4.6908221159999997</v>
       </c>
       <c r="G11" s="4">
+        <v>3.94889385657005</v>
+      </c>
+      <c r="H11" s="4">
         <v>0.36499999999999999</v>
       </c>
-      <c r="H11" s="4">
-        <v>1</v>
-      </c>
       <c r="I11" s="4">
         <v>1</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -943,48 +982,54 @@
         <v>4.7698549300000002</v>
       </c>
       <c r="G12" s="4">
+        <v>3.7559214080558898</v>
+      </c>
+      <c r="H12" s="4">
         <v>0.26700000000000002</v>
       </c>
-      <c r="H12" s="4">
+      <c r="I12" s="4">
         <v>9</v>
       </c>
-      <c r="I12" s="4">
+      <c r="J12" s="4">
         <v>0.3</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="6">
         <v>4854</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="6">
         <v>31</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="6">
         <v>8.1747019999999999</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="6">
         <v>6.8127316999999996</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="6">
         <v>1.199915329</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="6">
+        <v>0.45016418100655797</v>
+      </c>
+      <c r="H13" s="6">
         <v>0.58399999999999996</v>
       </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1004,7 +1049,7 @@
         <v>5.2669669350000001</v>
       </c>
       <c r="G14" s="4">
-        <v>1</v>
+        <v>5.6852364758188099</v>
       </c>
       <c r="H14" s="4">
         <v>1</v>
@@ -1012,11 +1057,14 @@
       <c r="I14" s="4">
         <v>1</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="4">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1036,16 +1084,19 @@
         <v>2.665813816</v>
       </c>
       <c r="G15" s="2">
+        <v>4.0320583473424003</v>
+      </c>
+      <c r="H15" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
       <c r="I15" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1065,19 +1116,22 @@
         <v>3.5777605819999998</v>
       </c>
       <c r="G16" s="4">
+        <v>3.0058423905198799</v>
+      </c>
+      <c r="H16" s="4">
         <v>0.54920000000000002</v>
       </c>
-      <c r="H16" s="4">
-        <v>1</v>
-      </c>
       <c r="I16" s="4">
         <v>1</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1097,16 +1151,19 @@
         <v>2.5714123359999999</v>
       </c>
       <c r="G17" s="2">
+        <v>2.3385963505407501</v>
+      </c>
+      <c r="H17" s="2">
         <v>0.45</v>
       </c>
-      <c r="H17" s="2">
-        <v>0</v>
-      </c>
       <c r="I17" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1126,16 +1183,19 @@
         <v>4.8056964940000002</v>
       </c>
       <c r="G18" s="2">
+        <v>7.6809675862101097</v>
+      </c>
+      <c r="H18" s="2">
         <v>0.54</v>
       </c>
-      <c r="H18" s="2">
-        <v>0</v>
-      </c>
       <c r="I18" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -1155,51 +1215,57 @@
         <v>2.2409054780000002</v>
       </c>
       <c r="G19" s="4">
-        <v>1</v>
+        <v>1.3956972394666101</v>
       </c>
       <c r="H19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="4">
         <v>0</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
-        <v>5000</v>
-      </c>
-      <c r="C20" s="6">
+      <c r="B20" s="12">
+        <v>5000</v>
+      </c>
+      <c r="C20" s="12">
         <v>2546</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="12">
         <v>12.079599999999999</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="12">
         <v>10.855600000000001</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="12">
         <v>1.112752865</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="12">
+        <v>0.40936638020986099</v>
+      </c>
+      <c r="H20" s="12">
         <v>0.90200000000000002</v>
       </c>
-      <c r="H20" s="6">
+      <c r="I20" s="12">
         <v>6</v>
       </c>
-      <c r="I20" s="6">
-        <v>1</v>
-      </c>
-      <c r="J20" s="7" t="s">
+      <c r="J20" s="12">
+        <v>1</v>
+      </c>
+      <c r="K20" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1219,77 +1285,86 @@
         <v>2.3552507770000002</v>
       </c>
       <c r="G21" s="4">
+        <v>1.78980835509714</v>
+      </c>
+      <c r="H21" s="4">
         <v>0.12</v>
       </c>
-      <c r="H21" s="4">
+      <c r="I21" s="4">
         <v>2</v>
       </c>
-      <c r="I21" s="4">
+      <c r="J21" s="4">
         <v>0.8</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="K21" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
-        <v>5000</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="B22" s="12">
+        <v>5000</v>
+      </c>
+      <c r="C22" s="12">
         <v>400</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="12">
         <v>8.2306000000000008</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="12">
         <v>7.1929999999999996</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="12">
         <v>1.144251355</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="12">
+        <v>0.37839703644484601</v>
+      </c>
+      <c r="H22" s="12">
         <v>0.35799999999999998</v>
       </c>
-      <c r="H22" s="2">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="I22" s="12">
+        <v>1</v>
+      </c>
+      <c r="J22" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
-        <v>5000</v>
-      </c>
-      <c r="C23" s="2">
+      <c r="B23" s="12">
+        <v>5000</v>
+      </c>
+      <c r="C23" s="12">
         <v>27</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="12">
         <v>42.176200000000001</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="12">
         <v>12.7918</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="12">
         <v>3.2971278480000001</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="12">
+        <v>5.9155014869004798</v>
+      </c>
+      <c r="H23" s="12">
         <v>0.51900000000000002</v>
       </c>
-      <c r="H23" s="2">
-        <v>1</v>
-      </c>
-      <c r="I23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I23" s="12">
+        <v>0</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1309,12 +1384,15 @@
         <v>2.375155876</v>
       </c>
       <c r="G24" s="2">
+        <v>1.8413548800206601</v>
+      </c>
+      <c r="H24" s="2">
         <v>0.23</v>
       </c>
-      <c r="H24" s="2">
-        <v>0</v>
-      </c>
       <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
still studying the parameters on excell
</commit_message>
<xml_diff>
--- a/executions-best-parameters.xlsx
+++ b/executions-best-parameters.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Dataset</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>minPredictionRatio = [5,10]</t>
+  </si>
+  <si>
+    <t>#splitLength</t>
   </si>
 </sst>
 </file>
@@ -734,11 +737,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -748,16 +751,16 @@
     <col min="4" max="4" width="10.83203125" style="31"/>
     <col min="5" max="5" width="17.5" style="31" customWidth="1"/>
     <col min="6" max="7" width="33.83203125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="17.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="12" width="18.5" style="1" customWidth="1"/>
-    <col min="13" max="14" width="10.83203125" style="1"/>
-    <col min="15" max="15" width="40.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="10" width="17.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="18.5" style="1" customWidth="1"/>
+    <col min="14" max="15" width="10.83203125" style="1"/>
+    <col min="16" max="16" width="40.33203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -786,22 +789,25 @@
         <v>48</v>
       </c>
       <c r="J1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -830,13 +836,13 @@
         <v>1</v>
       </c>
       <c r="J2" s="8">
+        <v>10</v>
+      </c>
+      <c r="K2" s="8">
         <v>3</v>
       </c>
-      <c r="K2" s="8">
-        <v>1</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>51</v>
+      <c r="L2" s="8">
+        <v>1</v>
       </c>
       <c r="M2" s="17" t="s">
         <v>51</v>
@@ -844,11 +850,14 @@
       <c r="N2" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -876,14 +885,14 @@
       <c r="I3" s="8">
         <v>1</v>
       </c>
-      <c r="J3" s="9">
-        <v>1</v>
+      <c r="J3" s="8">
+        <v>20</v>
       </c>
       <c r="K3" s="9">
         <v>1</v>
       </c>
-      <c r="L3" s="17" t="s">
-        <v>51</v>
+      <c r="L3" s="9">
+        <v>1</v>
       </c>
       <c r="M3" s="17" t="s">
         <v>51</v>
@@ -891,11 +900,14 @@
       <c r="N3" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -923,23 +935,26 @@
       <c r="I4" s="8">
         <v>1</v>
       </c>
-      <c r="J4" s="9">
-        <v>0</v>
+      <c r="J4" s="8">
+        <v>6</v>
       </c>
       <c r="K4" s="9">
         <v>0</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="17">
         <v>0.55600000000000005</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>51</v>
       </c>
       <c r="N4" s="17" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="O4" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -967,26 +982,29 @@
       <c r="I5" s="8">
         <v>1</v>
       </c>
-      <c r="J5" s="9">
-        <v>1</v>
+      <c r="J5" s="8">
+        <v>6</v>
       </c>
       <c r="K5" s="9">
         <v>1</v>
       </c>
-      <c r="L5" s="19">
+      <c r="L5" s="9">
+        <v>1</v>
+      </c>
+      <c r="M5" s="19">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M5" s="17">
-        <v>0</v>
-      </c>
       <c r="N5" s="17">
         <v>0</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="17">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
@@ -1014,26 +1032,29 @@
       <c r="I6" s="8">
         <v>1</v>
       </c>
-      <c r="J6" s="10">
-        <v>0</v>
+      <c r="J6" s="8">
+        <v>8</v>
       </c>
       <c r="K6" s="10">
         <v>0</v>
       </c>
-      <c r="L6" s="19">
+      <c r="L6" s="10">
+        <v>0</v>
+      </c>
+      <c r="M6" s="19">
         <v>1.6E-2</v>
       </c>
-      <c r="M6" s="17">
-        <v>0</v>
-      </c>
       <c r="N6" s="17">
+        <v>0</v>
+      </c>
+      <c r="O6" s="17">
         <v>0.7</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>6</v>
       </c>
@@ -1061,26 +1082,29 @@
       <c r="I7" s="8">
         <v>1</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="8">
+        <v>22</v>
+      </c>
+      <c r="K7" s="10">
         <v>2</v>
       </c>
-      <c r="K7" s="10">
-        <v>1</v>
-      </c>
-      <c r="L7" s="17">
+      <c r="L7" s="10">
+        <v>1</v>
+      </c>
+      <c r="M7" s="17">
         <v>0.4</v>
       </c>
-      <c r="M7" s="19">
+      <c r="N7" s="19">
         <v>5</v>
       </c>
-      <c r="N7" s="17" t="s">
+      <c r="O7" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -1108,23 +1132,26 @@
       <c r="I8" s="8">
         <v>1</v>
       </c>
-      <c r="J8" s="9">
-        <v>1</v>
+      <c r="J8" s="8">
+        <v>12</v>
       </c>
       <c r="K8" s="9">
         <v>1</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="9">
+        <v>1</v>
+      </c>
+      <c r="M8" s="19">
         <v>0.21199999999999999</v>
       </c>
-      <c r="M8" s="17">
+      <c r="N8" s="17">
         <v>2</v>
       </c>
-      <c r="N8" s="17" t="s">
+      <c r="O8" s="17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1152,20 +1179,23 @@
       <c r="I9" s="8">
         <v>1</v>
       </c>
-      <c r="J9" s="11">
-        <v>1</v>
+      <c r="J9" s="8">
+        <v>22</v>
       </c>
       <c r="K9" s="11">
         <v>1</v>
       </c>
-      <c r="L9" s="18"/>
+      <c r="L9" s="11">
+        <v>1</v>
+      </c>
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="18"/>
+      <c r="P9" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1193,20 +1223,23 @@
       <c r="I10" s="8">
         <v>1</v>
       </c>
-      <c r="J10" s="11">
-        <v>1</v>
+      <c r="J10" s="8">
+        <v>22</v>
       </c>
       <c r="K10" s="11">
         <v>1</v>
       </c>
-      <c r="L10" s="18"/>
+      <c r="L10" s="11">
+        <v>1</v>
+      </c>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="18"/>
+      <c r="P10" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1234,20 +1267,23 @@
       <c r="I11" s="8">
         <v>1</v>
       </c>
-      <c r="J11" s="11">
-        <v>1</v>
+      <c r="J11" s="8">
+        <v>22</v>
       </c>
       <c r="K11" s="11">
         <v>1</v>
       </c>
-      <c r="L11" s="18"/>
+      <c r="L11" s="11">
+        <v>1</v>
+      </c>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="18"/>
+      <c r="P11" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1275,20 +1311,23 @@
       <c r="I12" s="8">
         <v>1</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="8">
+        <v>22</v>
+      </c>
+      <c r="K12" s="11">
         <v>9</v>
       </c>
-      <c r="K12" s="11">
+      <c r="L12" s="11">
         <v>0.3</v>
       </c>
-      <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="18"/>
+      <c r="P12" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>12</v>
       </c>
@@ -1316,20 +1355,23 @@
       <c r="I13" s="8">
         <v>1</v>
       </c>
-      <c r="J13" s="12">
-        <v>0</v>
+      <c r="J13" s="8">
+        <v>22</v>
       </c>
       <c r="K13" s="12">
         <v>0</v>
       </c>
-      <c r="L13" s="17"/>
+      <c r="L13" s="12">
+        <v>0</v>
+      </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
-      <c r="O13" s="5" t="s">
+      <c r="O13" s="17"/>
+      <c r="P13" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -1357,20 +1399,23 @@
       <c r="I14" s="8">
         <v>1</v>
       </c>
-      <c r="J14" s="11">
-        <v>1</v>
+      <c r="J14" s="8">
+        <v>22</v>
       </c>
       <c r="K14" s="11">
         <v>1</v>
       </c>
-      <c r="L14" s="18"/>
+      <c r="L14" s="11">
+        <v>1</v>
+      </c>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="18"/>
+      <c r="P14" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -1398,17 +1443,20 @@
       <c r="I15" s="8">
         <v>1</v>
       </c>
-      <c r="J15" s="9">
-        <v>0</v>
+      <c r="J15" s="8">
+        <v>22</v>
       </c>
       <c r="K15" s="9">
         <v>0</v>
       </c>
-      <c r="L15" s="17"/>
+      <c r="L15" s="9">
+        <v>0</v>
+      </c>
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
-    </row>
-    <row r="16" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O15" s="17"/>
+    </row>
+    <row r="16" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
@@ -1436,20 +1484,23 @@
       <c r="I16" s="8">
         <v>1</v>
       </c>
-      <c r="J16" s="11">
-        <v>1</v>
+      <c r="J16" s="8">
+        <v>22</v>
       </c>
       <c r="K16" s="11">
         <v>1</v>
       </c>
-      <c r="L16" s="18"/>
+      <c r="L16" s="11">
+        <v>1</v>
+      </c>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="4" t="s">
+      <c r="O16" s="18"/>
+      <c r="P16" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
@@ -1477,19 +1528,22 @@
       <c r="I17" s="8">
         <v>1</v>
       </c>
-      <c r="J17" s="9">
-        <v>0</v>
+      <c r="J17" s="8">
+        <v>22</v>
       </c>
       <c r="K17" s="9">
         <v>0</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="9">
+        <v>0</v>
+      </c>
+      <c r="M17" s="19">
         <v>0.38300000000000001</v>
       </c>
-      <c r="M17" s="17"/>
       <c r="N17" s="17"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O17" s="17"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -1517,19 +1571,22 @@
       <c r="I18" s="8">
         <v>1</v>
       </c>
-      <c r="J18" s="9">
-        <v>0</v>
+      <c r="J18" s="8">
+        <v>22</v>
       </c>
       <c r="K18" s="9">
         <v>0</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="9">
+        <v>0</v>
+      </c>
+      <c r="M18" s="19">
         <v>0.48099999999999998</v>
       </c>
-      <c r="M18" s="17"/>
       <c r="N18" s="17"/>
-    </row>
-    <row r="19" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O18" s="17"/>
+    </row>
+    <row r="19" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -1557,22 +1614,25 @@
       <c r="I19" s="8">
         <v>1</v>
       </c>
-      <c r="J19" s="11">
-        <v>0</v>
+      <c r="J19" s="8">
+        <v>22</v>
       </c>
       <c r="K19" s="11">
         <v>0</v>
       </c>
-      <c r="L19" s="20">
+      <c r="L19" s="11">
+        <v>0</v>
+      </c>
+      <c r="M19" s="20">
         <v>0.49199999999999999</v>
       </c>
-      <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="4" t="s">
+      <c r="O19" s="18"/>
+      <c r="P19" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>19</v>
       </c>
@@ -1601,19 +1661,22 @@
         <v>1</v>
       </c>
       <c r="J20" s="8">
+        <v>22</v>
+      </c>
+      <c r="K20" s="8">
         <v>6</v>
       </c>
-      <c r="K20" s="8">
-        <v>1</v>
-      </c>
-      <c r="L20" s="17"/>
+      <c r="L20" s="8">
+        <v>1</v>
+      </c>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
-      <c r="O20" s="6" t="s">
+      <c r="O20" s="17"/>
+      <c r="P20" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -1641,20 +1704,23 @@
       <c r="I21" s="8">
         <v>1</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J21" s="8">
+        <v>22</v>
+      </c>
+      <c r="K21" s="11">
         <v>2</v>
       </c>
-      <c r="K21" s="11">
+      <c r="L21" s="11">
         <v>0.8</v>
       </c>
-      <c r="L21" s="18"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
-      <c r="O21" s="4" t="s">
+      <c r="O21" s="18"/>
+      <c r="P21" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>21</v>
       </c>
@@ -1683,16 +1749,19 @@
         <v>1</v>
       </c>
       <c r="J22" s="8">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="K22" s="8">
         <v>1</v>
       </c>
-      <c r="L22" s="17"/>
+      <c r="L22" s="8">
+        <v>1</v>
+      </c>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
-    </row>
-    <row r="23" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O22" s="17"/>
+    </row>
+    <row r="23" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>22</v>
       </c>
@@ -1721,18 +1790,21 @@
         <v>1</v>
       </c>
       <c r="J23" s="8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K23" s="8">
         <v>0</v>
       </c>
-      <c r="L23" s="19">
+      <c r="L23" s="8">
+        <v>0</v>
+      </c>
+      <c r="M23" s="19">
         <v>0.30499999999999999</v>
       </c>
-      <c r="M23" s="17"/>
       <c r="N23" s="17"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O23" s="17"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>23</v>
       </c>
@@ -1760,54 +1832,57 @@
       <c r="I24" s="8">
         <v>1</v>
       </c>
-      <c r="J24" s="9">
-        <v>0</v>
+      <c r="J24" s="8">
+        <v>22</v>
       </c>
       <c r="K24" s="9">
         <v>0</v>
       </c>
-      <c r="L24" s="19">
+      <c r="L24" s="9">
+        <v>0</v>
+      </c>
+      <c r="M24" s="19">
         <v>0.16900000000000001</v>
       </c>
-      <c r="M24" s="17"/>
       <c r="N24" s="17"/>
-    </row>
-    <row r="27" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O24" s="17"/>
+    </row>
+    <row r="27" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
         <v>43</v>
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
     </row>
-    <row r="28" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
     </row>
-    <row r="29" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
         <v>41</v>
       </c>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
     </row>
-    <row r="30" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
         <v>47</v>
       </c>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
     </row>
-    <row r="31" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
         <v>42</v>
       </c>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
     </row>
-    <row r="32" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
         <v>44</v>
       </c>

</xml_diff>